<commit_message>
add new version learn model with frontend
</commit_message>
<xml_diff>
--- a/lab3/lab3.xlsx
+++ b/lab3/lab3.xlsx
@@ -67,7 +67,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -89,12 +89,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -392,45 +386,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:t>Заглавие диаграммы</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
@@ -742,6 +702,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -927,11 +888,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="75588452"/>
-        <c:axId val="78362509"/>
+        <c:axId val="46902865"/>
+        <c:axId val="26241760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75588452"/>
+        <c:axId val="46902865"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -973,12 +934,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78362509"/>
+        <c:crossAx val="26241760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78362509"/>
+        <c:axId val="26241760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +981,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75588452"/>
+        <c:crossAx val="46902865"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1050,45 +1011,11 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:t>Заглавие диаграммы</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:scatterChart>
@@ -1215,11 +1142,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42612219"/>
-        <c:axId val="21384233"/>
+        <c:axId val="73767411"/>
+        <c:axId val="25423518"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42612219"/>
+        <c:axId val="73767411"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1261,12 +1188,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21384233"/>
+        <c:crossAx val="25423518"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21384233"/>
+        <c:axId val="25423518"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1235,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42612219"/>
+        <c:crossAx val="73767411"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1347,9 +1274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>454320</xdr:colOff>
+      <xdr:colOff>453960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1357,8 +1284,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12885120" y="2251080"/>
-        <a:ext cx="6957360" cy="4091040"/>
+        <a:off x="12893040" y="2251080"/>
+        <a:ext cx="6961320" cy="4090680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1377,9 +1304,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>690480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1387,8 +1314,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20653560" y="4179240"/>
-        <a:ext cx="5548320" cy="2732760"/>
+        <a:off x="20666160" y="4179240"/>
+        <a:ext cx="5551200" cy="2732400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1407,9 +1334,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>106920</xdr:colOff>
+      <xdr:colOff>106560</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1422,8 +1349,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2253960" y="117000"/>
-          <a:ext cx="4995720" cy="3534480"/>
+          <a:off x="2255040" y="117000"/>
+          <a:ext cx="4998960" cy="3534120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1446,10 +1373,10 @@
   <dimension ref="C27:P77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">

</xml_diff>